<commit_message>
FabriLife Test Report Done
</commit_message>
<xml_diff>
--- a/FabriLife_Test-Case-Report.xlsx
+++ b/FabriLife_Test-Case-Report.xlsx
@@ -2818,7 +2818,9 @@
       </c>
       <c r="X2" s="2"/>
       <c r="Y2" s="3"/>
-      <c r="Z2" s="10"/>
+      <c r="Z2" s="8">
+        <v>42.0</v>
+      </c>
       <c r="AA2" s="2"/>
       <c r="AB2" s="3"/>
     </row>
@@ -2860,7 +2862,9 @@
       </c>
       <c r="X3" s="2"/>
       <c r="Y3" s="3"/>
-      <c r="Z3" s="10"/>
+      <c r="Z3" s="8">
+        <v>11.0</v>
+      </c>
       <c r="AA3" s="2"/>
       <c r="AB3" s="3"/>
     </row>
@@ -2900,7 +2904,9 @@
       </c>
       <c r="X4" s="2"/>
       <c r="Y4" s="3"/>
-      <c r="Z4" s="10"/>
+      <c r="Z4" s="8">
+        <v>0.0</v>
+      </c>
       <c r="AA4" s="2"/>
       <c r="AB4" s="3"/>
     </row>
@@ -2936,7 +2942,9 @@
       </c>
       <c r="X5" s="2"/>
       <c r="Y5" s="3"/>
-      <c r="Z5" s="10"/>
+      <c r="Z5" s="8">
+        <v>0.0</v>
+      </c>
       <c r="AA5" s="2"/>
       <c r="AB5" s="3"/>
     </row>
@@ -2968,7 +2976,9 @@
       </c>
       <c r="X6" s="2"/>
       <c r="Y6" s="3"/>
-      <c r="Z6" s="10"/>
+      <c r="Z6" s="8">
+        <v>53.0</v>
+      </c>
       <c r="AA6" s="2"/>
       <c r="AB6" s="3"/>
     </row>
@@ -3274,7 +3284,7 @@
       <c r="BJ11" s="17"/>
       <c r="BK11" s="18"/>
     </row>
-    <row r="12" ht="39.75" customHeight="1">
+    <row r="12" ht="30.75" customHeight="1">
       <c r="A12" s="21"/>
       <c r="B12" s="23"/>
       <c r="C12" s="21"/>
@@ -3489,7 +3499,7 @@
       <c r="BJ14" s="17"/>
       <c r="BK14" s="18"/>
     </row>
-    <row r="15" ht="51.75" customHeight="1">
+    <row r="15" ht="30.0" customHeight="1">
       <c r="A15" s="21"/>
       <c r="B15" s="23"/>
       <c r="C15" s="34"/>
@@ -3627,7 +3637,7 @@
       <c r="BJ16" s="17"/>
       <c r="BK16" s="18"/>
     </row>
-    <row r="17" ht="42.0" customHeight="1">
+    <row r="17" ht="24.0" customHeight="1">
       <c r="A17" s="21"/>
       <c r="B17" s="23"/>
       <c r="C17" s="34"/>
@@ -3765,7 +3775,7 @@
       <c r="BJ18" s="17"/>
       <c r="BK18" s="18"/>
     </row>
-    <row r="19" ht="35.25" customHeight="1">
+    <row r="19" ht="21.75" customHeight="1">
       <c r="A19" s="21"/>
       <c r="B19" s="23"/>
       <c r="C19" s="34"/>
@@ -3903,7 +3913,7 @@
       <c r="BJ20" s="17"/>
       <c r="BK20" s="18"/>
     </row>
-    <row r="21" ht="30.0" customHeight="1">
+    <row r="21" ht="21.0" customHeight="1">
       <c r="A21" s="21"/>
       <c r="B21" s="23"/>
       <c r="C21" s="34"/>
@@ -4041,7 +4051,7 @@
       <c r="BJ22" s="17"/>
       <c r="BK22" s="18"/>
     </row>
-    <row r="23" ht="36.75" customHeight="1">
+    <row r="23" ht="25.5" customHeight="1">
       <c r="A23" s="21"/>
       <c r="B23" s="23"/>
       <c r="C23" s="34"/>
@@ -4103,7 +4113,7 @@
       <c r="BJ23" s="22"/>
       <c r="BK23" s="23"/>
     </row>
-    <row r="24" ht="46.5" customHeight="1">
+    <row r="24" ht="36.0" customHeight="1">
       <c r="A24" s="8">
         <v>7.0</v>
       </c>
@@ -4327,7 +4337,7 @@
       <c r="BJ26" s="17"/>
       <c r="BK26" s="18"/>
     </row>
-    <row r="27" ht="27.75" customHeight="1">
+    <row r="27" ht="26.25" customHeight="1">
       <c r="A27" s="21"/>
       <c r="B27" s="23"/>
       <c r="C27" s="34"/>
@@ -4465,7 +4475,7 @@
       <c r="BJ28" s="17"/>
       <c r="BK28" s="18"/>
     </row>
-    <row r="29" ht="24.75" customHeight="1">
+    <row r="29" ht="23.25" customHeight="1">
       <c r="A29" s="21"/>
       <c r="B29" s="23"/>
       <c r="C29" s="34"/>
@@ -4605,7 +4615,7 @@
       <c r="BJ30" s="17"/>
       <c r="BK30" s="18"/>
     </row>
-    <row r="31" ht="27.0" customHeight="1">
+    <row r="31" ht="32.25" customHeight="1">
       <c r="A31" s="21"/>
       <c r="B31" s="23"/>
       <c r="C31" s="34"/>
@@ -5441,7 +5451,7 @@
       <c r="BJ42" s="17"/>
       <c r="BK42" s="18"/>
     </row>
-    <row r="43" ht="24.75" customHeight="1">
+    <row r="43" ht="30.75" customHeight="1">
       <c r="A43" s="21"/>
       <c r="B43" s="23"/>
       <c r="C43" s="34"/>
@@ -5579,7 +5589,7 @@
       <c r="BJ44" s="17"/>
       <c r="BK44" s="18"/>
     </row>
-    <row r="45" ht="24.75" customHeight="1">
+    <row r="45" ht="30.0" customHeight="1">
       <c r="A45" s="21"/>
       <c r="B45" s="23"/>
       <c r="C45" s="34"/>
@@ -9313,7 +9323,7 @@
       <c r="BJ98" s="17"/>
       <c r="BK98" s="18"/>
     </row>
-    <row r="99" ht="23.25" customHeight="1">
+    <row r="99" ht="27.75" customHeight="1">
       <c r="A99" s="21"/>
       <c r="B99" s="23"/>
       <c r="C99" s="34"/>
@@ -10145,7 +10155,7 @@
       <c r="BJ110" s="17"/>
       <c r="BK110" s="18"/>
     </row>
-    <row r="111" ht="19.5" customHeight="1">
+    <row r="111" ht="25.5" customHeight="1">
       <c r="A111" s="21"/>
       <c r="B111" s="23"/>
       <c r="C111" s="34"/>
@@ -10283,7 +10293,7 @@
       <c r="BJ112" s="17"/>
       <c r="BK112" s="18"/>
     </row>
-    <row r="113" ht="23.25" customHeight="1">
+    <row r="113" ht="33.0" customHeight="1">
       <c r="A113" s="21"/>
       <c r="B113" s="23"/>
       <c r="C113" s="34"/>
@@ -10423,7 +10433,7 @@
       <c r="BJ114" s="17"/>
       <c r="BK114" s="18"/>
     </row>
-    <row r="115" ht="22.5" customHeight="1">
+    <row r="115" ht="29.25" customHeight="1">
       <c r="A115" s="21"/>
       <c r="B115" s="23"/>
       <c r="C115" s="34"/>
@@ -10561,7 +10571,7 @@
       <c r="BJ116" s="17"/>
       <c r="BK116" s="18"/>
     </row>
-    <row r="117" ht="24.0" customHeight="1">
+    <row r="117" ht="33.75" customHeight="1">
       <c r="A117" s="21"/>
       <c r="B117" s="23"/>
       <c r="C117" s="21"/>

</xml_diff>